<commit_message>
Work on global rec strategies
</commit_message>
<xml_diff>
--- a/evals/als_excel.xlsx
+++ b/evals/als_excel.xlsx
@@ -4491,7 +4491,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -9177,7 +9177,7 @@
   <dimension ref="B1:M112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+      <selection activeCell="O115" sqref="O115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
backup prior to final experiment
</commit_message>
<xml_diff>
--- a/evals/als_excel.xlsx
+++ b/evals/als_excel.xlsx
@@ -9,25 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="23540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALS" sheetId="3" r:id="rId1"/>
     <sheet name="stromy" sheetId="6" r:id="rId2"/>
     <sheet name="rf pivot" sheetId="8" r:id="rId3"/>
     <sheet name="rf" sheetId="7" r:id="rId4"/>
-    <sheet name="Popularita PLISTA" sheetId="5" r:id="rId5"/>
-    <sheet name="KMEANS" sheetId="4" r:id="rId6"/>
+    <sheet name="gbts" sheetId="9" r:id="rId5"/>
+    <sheet name="Popularita PLISTA" sheetId="5" r:id="rId6"/>
+    <sheet name="KMEANS" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">rf!$B$1:$D$281</definedName>
     <definedName name="file" localSheetId="0">ALS!$B$2:$F$57</definedName>
-    <definedName name="file_1" localSheetId="5">KMEANS!$B$2:$E$209</definedName>
+    <definedName name="file_1" localSheetId="6">KMEANS!$B$2:$E$209</definedName>
+    <definedName name="file_gbt" localSheetId="4">gbts!#REF!</definedName>
+    <definedName name="file_gbt_1" localSheetId="4">gbts!$A$2:$E$90</definedName>
     <definedName name="file_rf_1" localSheetId="3">rf!$A$2:$E$141</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -50,7 +53,29 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="file_rf" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" name="file_gbt" type="6" refreshedVersion="0" background="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Adam/PycharmProjects/scarec/evals/file_gbt.csv" thousands=" " comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="file_gbt1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Adam/PycharmProjects/scarec/evals/file_gbt.csv" thousands=" " comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="file_rf" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Adam/PycharmProjects/scarec/evals/file_rf.csv" thousands=" " comma="1">
       <textFields count="5">
         <textField/>
@@ -61,7 +86,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="file1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="file1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Adam/Movies/file.csv" thousands=" " comma="1">
       <textFields count="4">
         <textField/>
@@ -75,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="773">
   <si>
     <t>TIME_TAKEN</t>
   </si>
@@ -1854,6 +1879,546 @@
   </si>
   <si>
     <t>tc:30:d:3</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_40_d_3cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:40:d:3</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_20cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:20</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_3cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:3</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_30cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:30</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_8cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:8</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_7cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:7</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_3cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:3</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_8cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:8</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_6cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:6</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_6cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:6</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_25cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:25</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_12cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:12</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_15cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:15</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_3cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:3</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_6cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:6</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_20cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:20</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_8cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:8</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_30cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:30</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_30cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:30</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_9cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:9</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_6cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:6</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_3cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:3</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_12cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:12</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_9cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:9</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_12cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:12</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_15cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:15</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_8cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:8</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_12cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:12</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_8cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:8</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_20cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:20</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_3cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:3</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_9cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:9</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_30cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:30</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_6cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:6</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_20cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:20</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_30cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:30</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_3cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:3</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_40_d_12cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:40:d:12</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_30cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:30</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_25cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:25</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_25cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:25</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_9cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:9</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_25cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:25</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_15cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:15</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_9cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:9</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_15cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:15</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_25cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:25</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_30cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:30</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_15cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:15</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_7cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:7</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_20cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:20</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_8cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:8</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_40_d_8cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:40:d:8</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_20cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:20</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_7cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:7</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_30cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:30</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_25cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:25</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_6cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:6</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_6cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:6</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_40_d_7cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:40:d:7</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_7cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:7</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_7cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:7</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_7cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:7</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_20cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:20</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_12cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:12</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_15cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:15</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_25cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:25</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_25cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:25</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_8cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:8</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_40_d_6cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:40:d:6</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_3cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:3</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_8cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:8</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_25_d_12cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:25:d:12</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_15cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:15</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_3_d_9cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:3:d:9</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_30_d_6cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:30:d:6</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_9cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:9</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_6_d_7cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:6:d:7</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_20cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:20</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_15cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:15</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_12cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:12</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_9_d_9cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:9:d:9</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_15_d_12cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:15:d:12</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_12_d_7cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:12:d:7</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_40_d_9cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:40:d:9</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_20_d_3cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:20:d:3</t>
+  </si>
+  <si>
+    <t>iters</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_40_d_25cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:40:d:25</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_40_d_20cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:40:d:20</t>
+  </si>
+  <si>
+    <t>b'eval:gbt:gbt_model_ic_40_d_15cluster_id:3:mse:'</t>
+  </si>
+  <si>
+    <t>iters:40:d:15</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -1935,7 +2500,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1956,6 +2521,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1990,7 +2561,7 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="32">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2003,6 +2574,9 @@
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2015,6 +2589,9 @@
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
@@ -6284,7 +6861,7 @@
             </a:solidFill>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -7988,6 +8565,968 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sk-SK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Gradient Boosted Trees - MSE (Mean squared error)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0901606858166988"/>
+          <c:y val="0.0524440923516141"/>
+          <c:w val="0.904884983220618"/>
+          <c:h val="0.784377721954897"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MSE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="45"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="45"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.09106977211125"/>
+                  <c:y val="-0.502624865523218"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>MIN @ iters:40 depth:9</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>gbts!$E$2:$E$87</c:f>
+              <c:strCache>
+                <c:ptCount val="86"/>
+                <c:pt idx="0">
+                  <c:v>iters:3:d:3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>iters:3:d:6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iters:3:d:7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>iters:3:d:8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>iters:3:d:9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>iters:3:d:12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>iters:3:d:15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>iters:3:d:20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>iters:3:d:25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>iters:3:d:30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>iters:6:d:3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>iters:6:d:6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>iters:6:d:7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>iters:6:d:8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>iters:6:d:9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>iters:6:d:12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>iters:6:d:15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>iters:6:d:20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>iters:6:d:25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>iters:6:d:30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>iters:9:d:3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>iters:9:d:6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>iters:9:d:7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>iters:9:d:8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>iters:9:d:9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>iters:9:d:12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>iters:9:d:15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>iters:9:d:20</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>iters:9:d:25</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>iters:9:d:30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>iters:12:d:3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>iters:12:d:6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>iters:12:d:7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>iters:12:d:8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>iters:12:d:9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>iters:12:d:12</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>iters:12:d:15</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>iters:12:d:20</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>iters:12:d:25</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>iters:12:d:30</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>iters:15:d:3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>iters:15:d:6</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>iters:15:d:7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>iters:15:d:8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>iters:15:d:9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>iters:15:d:12</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>iters:15:d:15</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>iters:15:d:20</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>iters:15:d:25</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>iters:15:d:30</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>iters:20:d:3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>iters:20:d:6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>iters:20:d:7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>iters:20:d:8</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>iters:20:d:9</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>iters:20:d:12</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>iters:20:d:15</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>iters:20:d:20</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>iters:20:d:25</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>iters:20:d:30</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>iters:25:d:3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>iters:25:d:6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>iters:25:d:7</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>iters:25:d:8</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>iters:25:d:9</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>iters:25:d:12</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>iters:25:d:15</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>iters:25:d:20</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>iters:25:d:25</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>iters:25:d:30</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>iters:30:d:3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>iters:30:d:6</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>iters:30:d:7</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>iters:30:d:8</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>iters:30:d:9</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>iters:30:d:12</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>iters:30:d:15</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>iters:30:d:20</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>iters:30:d:25</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>iters:30:d:30</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>iters:40:d:3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>iters:40:d:6</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>iters:40:d:7</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>iters:40:d:8</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>iters:40:d:9</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>iters:40:d:12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>gbts!$D$2:$D$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="86"/>
+                <c:pt idx="0">
+                  <c:v>0.22545657762335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.223100218503665</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.222794233002695</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.222590413945737</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.222378899324049</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.222021751168922</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.221877226300508</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.221630331181328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.221502868888678</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.221422203711636</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.224788360589679</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.222609587183102</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.222326058821376</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.222157907400749</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.222013819521554</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.221778322454007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.221614955483166</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.221477931546948</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.221382327334188</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.221312938527853</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.224113445715442</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.222308918827156</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.222097056845976</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.221940272736853</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.221819483963415</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.221599171548624</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.221527374645629</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.221409923700609</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.221335690353357</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.221264777288636</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.223825533016111</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.222147803525383</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.221951589020362</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.221770210384906</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.221674373120043</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.221497651088186</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.22144283859842</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.221360916283074</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.221311384931444</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.221251520525102</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.223487639975396</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.222003956854298</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.221807816586796</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.221689149610074</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.221561436531854</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.221422014688379</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.221364815685387</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.221318919420111</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.221306052274392</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.221244937237576</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.223198704259315</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.221817933593109</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.221662024744538</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.221545365946234</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.221455319746652</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.221345927442884</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.221348576730321</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.221295033164883</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.221256048425515</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.221266789138689</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.222795031941381</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.221693782783812</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.221552559054129</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.221434108197833</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.221361014756824</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.221277565853437</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.221300228384552</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.221283491745269</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.221250268557251</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.221254066623265</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.222640372164842</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.221595483949434</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.221476322624508</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.221368596176375</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.221302682765161</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.221252006516487</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.221253796904716</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.221271705670319</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.221243925418516</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.221240522486206</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.222364501700707</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.221462298605544</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.221372305522444</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.221292913861083</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.221235022268316</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.221224852155521</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1445749920"/>
+        <c:axId val="-2072564288"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1445749920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2072564288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2072564288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.228"/>
+          <c:min val="0.219"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>MSE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1445749920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="sk-SK"/>
@@ -8928,6 +10467,46 @@
 </file>
 
 <file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent4"/>
@@ -12418,6 +13997,509 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13083,15 +15165,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13123,8 +15205,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>277092</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>773545</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -13149,6 +15231,43 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>206663</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>70428</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -15169,11 +17288,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="file_rf_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="file_rf_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="file_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="file_gbt_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="file_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15453,10 +17576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M112"/>
+  <dimension ref="B1:N132"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="N132" sqref="N132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16598,6 +18721,11 @@
     </row>
     <row r="112" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M112" s="11"/>
+    </row>
+    <row r="132" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N132" t="s">
+        <v>772</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B2:F57">
@@ -17901,8 +20029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20326,16 +22454,1577 @@
     <sortCondition ref="C2:C141"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H90"/>
+  <sheetViews>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="N99" sqref="N99"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>733</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>0.22545657762335</v>
+      </c>
+      <c r="E2" t="s">
+        <v>734</v>
+      </c>
+      <c r="H2">
+        <f>MIN(D:D)</f>
+        <v>0.221205172193429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>621</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>0.22310021850366499</v>
+      </c>
+      <c r="E3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>603</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>0.22279423300269499</v>
+      </c>
+      <c r="E4" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>645</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>0.222590413945737</v>
+      </c>
+      <c r="E5" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>741</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>0.222378899324049</v>
+      </c>
+      <c r="E6" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>637</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>0.222021751168922</v>
+      </c>
+      <c r="E7" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>0.22187722630050799</v>
+      </c>
+      <c r="E8" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>719</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>0.22163033118132799</v>
+      </c>
+      <c r="E9" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>673</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>0.22150286888867801</v>
+      </c>
+      <c r="E10" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>669</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>0.22142220371163601</v>
+      </c>
+      <c r="E11" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>635</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0.22478836058967899</v>
+      </c>
+      <c r="E12" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>633</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>0.222609587183102</v>
+      </c>
+      <c r="E13" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>747</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>0.22232605882137599</v>
+      </c>
+      <c r="E14" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>601</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>0.22215790740074901</v>
+      </c>
+      <c r="E15" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>681</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>0.222013819521554</v>
+      </c>
+      <c r="E16" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>721</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>0.221778322454007</v>
+      </c>
+      <c r="E17" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>689</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>0.22161495548316601</v>
+      </c>
+      <c r="E18" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>651</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>0.221477931546948</v>
+      </c>
+      <c r="E19" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>613</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>0.221382327334188</v>
+      </c>
+      <c r="E20" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>629</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>0.221312938527853</v>
+      </c>
+      <c r="E21" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>597</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>0.22411344571544201</v>
+      </c>
+      <c r="E22" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>611</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>0.222308918827156</v>
+      </c>
+      <c r="E23" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>713</v>
+      </c>
+      <c r="B24">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>0.222097056845976</v>
+      </c>
+      <c r="E24" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>729</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>0.22194027273685299</v>
+      </c>
+      <c r="E25" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>755</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>0.221819483963415</v>
+      </c>
+      <c r="E26" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>615</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>0.22159917154862399</v>
+      </c>
+      <c r="E27" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>751</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>0.22152737464562899</v>
+      </c>
+      <c r="E28" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>623</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>0.221409923700609</v>
+      </c>
+      <c r="E29" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>705</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>25</v>
+      </c>
+      <c r="D30">
+        <v>0.22133569035335701</v>
+      </c>
+      <c r="E30" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>599</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>0.221264777288636</v>
+      </c>
+      <c r="E31" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>619</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>0.22382553301611099</v>
+      </c>
+      <c r="E32" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>659</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>0.22214780352538299</v>
+      </c>
+      <c r="E33" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>759</v>
+      </c>
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>0.22195158902036199</v>
+      </c>
+      <c r="E34" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>625</v>
+      </c>
+      <c r="B35">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>0.22177021038490599</v>
+      </c>
+      <c r="E35" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>655</v>
+      </c>
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+      <c r="D36">
+        <v>0.22167437312004301</v>
+      </c>
+      <c r="E36" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>647</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>0.221497651088186</v>
+      </c>
+      <c r="E37" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>679</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>15</v>
+      </c>
+      <c r="D38">
+        <v>0.22144283859842001</v>
+      </c>
+      <c r="E38" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>699</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>20</v>
+      </c>
+      <c r="D39">
+        <v>0.221360916283074</v>
+      </c>
+      <c r="E39" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>677</v>
+      </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>25</v>
+      </c>
+      <c r="D40">
+        <v>0.22131138493144401</v>
+      </c>
+      <c r="E40" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>657</v>
+      </c>
+      <c r="B41">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <v>30</v>
+      </c>
+      <c r="D41">
+        <v>0.221251520525102</v>
+      </c>
+      <c r="E41" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>665</v>
+      </c>
+      <c r="B42">
+        <v>15</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>0.223487639975396</v>
+      </c>
+      <c r="E42" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>707</v>
+      </c>
+      <c r="B43">
+        <v>15</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>0.222003956854298</v>
+      </c>
+      <c r="E43" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>715</v>
+      </c>
+      <c r="B44">
+        <v>15</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>0.22180781658679599</v>
+      </c>
+      <c r="E44" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>649</v>
+      </c>
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45">
+        <v>0.22168914961007399</v>
+      </c>
+      <c r="E45" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>631</v>
+      </c>
+      <c r="B46">
+        <v>15</v>
+      </c>
+      <c r="C46">
+        <v>9</v>
+      </c>
+      <c r="D46">
+        <v>0.22156143653185401</v>
+      </c>
+      <c r="E46" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>757</v>
+      </c>
+      <c r="B47">
+        <v>15</v>
+      </c>
+      <c r="C47">
+        <v>12</v>
+      </c>
+      <c r="D47">
+        <v>0.22142201468837899</v>
+      </c>
+      <c r="E47" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>643</v>
+      </c>
+      <c r="B48">
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>15</v>
+      </c>
+      <c r="D48">
+        <v>0.22136481568538699</v>
+      </c>
+      <c r="E48" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>749</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <v>20</v>
+      </c>
+      <c r="D49">
+        <v>0.221318919420111</v>
+      </c>
+      <c r="E49" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>725</v>
+      </c>
+      <c r="B50">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>25</v>
+      </c>
+      <c r="D50">
+        <v>0.22130605227439201</v>
+      </c>
+      <c r="E50" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>687</v>
+      </c>
+      <c r="B51">
+        <v>15</v>
+      </c>
+      <c r="C51">
+        <v>30</v>
+      </c>
+      <c r="D51">
+        <v>0.22124493723757599</v>
+      </c>
+      <c r="E51" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>763</v>
+      </c>
+      <c r="B52">
+        <v>20</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>0.22319870425931501</v>
+      </c>
+      <c r="E52" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>609</v>
+      </c>
+      <c r="B53">
+        <v>20</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <v>0.221817933593109</v>
+      </c>
+      <c r="E53" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>717</v>
+      </c>
+      <c r="B54">
+        <v>20</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <v>0.221662024744538</v>
+      </c>
+      <c r="E54" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>695</v>
+      </c>
+      <c r="B55">
+        <v>20</v>
+      </c>
+      <c r="C55">
+        <v>8</v>
+      </c>
+      <c r="D55">
+        <v>0.221545365946234</v>
+      </c>
+      <c r="E55" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>745</v>
+      </c>
+      <c r="B56">
+        <v>20</v>
+      </c>
+      <c r="C56">
+        <v>9</v>
+      </c>
+      <c r="D56">
+        <v>0.221455319746652</v>
+      </c>
+      <c r="E56" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>753</v>
+      </c>
+      <c r="B57">
+        <v>20</v>
+      </c>
+      <c r="C57">
+        <v>12</v>
+      </c>
+      <c r="D57">
+        <v>0.22134592744288401</v>
+      </c>
+      <c r="E57" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>739</v>
+      </c>
+      <c r="B58">
+        <v>20</v>
+      </c>
+      <c r="C58">
+        <v>15</v>
+      </c>
+      <c r="D58">
+        <v>0.22134857673032099</v>
+      </c>
+      <c r="E58" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>661</v>
+      </c>
+      <c r="B59">
+        <v>20</v>
+      </c>
+      <c r="C59">
+        <v>20</v>
+      </c>
+      <c r="D59">
+        <v>0.221295033164883</v>
+      </c>
+      <c r="E59" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>685</v>
+      </c>
+      <c r="B60">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>25</v>
+      </c>
+      <c r="D60">
+        <v>0.221256048425515</v>
+      </c>
+      <c r="E60" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>703</v>
+      </c>
+      <c r="B61">
+        <v>20</v>
+      </c>
+      <c r="C61">
+        <v>30</v>
+      </c>
+      <c r="D61">
+        <v>0.221266789138689</v>
+      </c>
+      <c r="E61" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>653</v>
+      </c>
+      <c r="B62">
+        <v>25</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>0.22279503194138101</v>
+      </c>
+      <c r="E62" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>709</v>
+      </c>
+      <c r="B63">
+        <v>25</v>
+      </c>
+      <c r="C63">
+        <v>6</v>
+      </c>
+      <c r="D63">
+        <v>0.22169378278381199</v>
+      </c>
+      <c r="E63" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>691</v>
+      </c>
+      <c r="B64">
+        <v>25</v>
+      </c>
+      <c r="C64">
+        <v>7</v>
+      </c>
+      <c r="D64">
+        <v>0.22155255905412899</v>
+      </c>
+      <c r="E64" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>607</v>
+      </c>
+      <c r="B65">
+        <v>25</v>
+      </c>
+      <c r="C65">
+        <v>8</v>
+      </c>
+      <c r="D65">
+        <v>0.22143410819783299</v>
+      </c>
+      <c r="E65" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>639</v>
+      </c>
+      <c r="B66">
+        <v>25</v>
+      </c>
+      <c r="C66">
+        <v>9</v>
+      </c>
+      <c r="D66">
+        <v>0.22136101475682399</v>
+      </c>
+      <c r="E66" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>737</v>
+      </c>
+      <c r="B67">
+        <v>25</v>
+      </c>
+      <c r="C67">
+        <v>12</v>
+      </c>
+      <c r="D67">
+        <v>0.221277565853437</v>
+      </c>
+      <c r="E67" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>683</v>
+      </c>
+      <c r="B68">
+        <v>25</v>
+      </c>
+      <c r="C68">
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <v>0.22130022838455199</v>
+      </c>
+      <c r="E68" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>595</v>
+      </c>
+      <c r="B69">
+        <v>25</v>
+      </c>
+      <c r="C69">
+        <v>20</v>
+      </c>
+      <c r="D69">
+        <v>0.22128349174526901</v>
+      </c>
+      <c r="E69" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>727</v>
+      </c>
+      <c r="B70">
+        <v>25</v>
+      </c>
+      <c r="C70">
+        <v>25</v>
+      </c>
+      <c r="D70">
+        <v>0.221250268557251</v>
+      </c>
+      <c r="E70" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>627</v>
+      </c>
+      <c r="B71">
+        <v>25</v>
+      </c>
+      <c r="C71">
+        <v>30</v>
+      </c>
+      <c r="D71">
+        <v>0.22125406662326499</v>
+      </c>
+      <c r="E71" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>605</v>
+      </c>
+      <c r="B72">
+        <v>30</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72">
+        <v>0.222640372164842</v>
+      </c>
+      <c r="E72" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>743</v>
+      </c>
+      <c r="B73">
+        <v>30</v>
+      </c>
+      <c r="C73">
+        <v>6</v>
+      </c>
+      <c r="D73">
+        <v>0.22159548394943401</v>
+      </c>
+      <c r="E73" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>701</v>
+      </c>
+      <c r="B74">
+        <v>30</v>
+      </c>
+      <c r="C74">
+        <v>7</v>
+      </c>
+      <c r="D74">
+        <v>0.221476322624508</v>
+      </c>
+      <c r="E74" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>735</v>
+      </c>
+      <c r="B75">
+        <v>30</v>
+      </c>
+      <c r="C75">
+        <v>8</v>
+      </c>
+      <c r="D75">
+        <v>0.221368596176375</v>
+      </c>
+      <c r="E75" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>675</v>
+      </c>
+      <c r="B76">
+        <v>30</v>
+      </c>
+      <c r="C76">
+        <v>9</v>
+      </c>
+      <c r="D76">
+        <v>0.22130268276516099</v>
+      </c>
+      <c r="E76" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>641</v>
+      </c>
+      <c r="B77">
+        <v>30</v>
+      </c>
+      <c r="C77">
+        <v>12</v>
+      </c>
+      <c r="D77">
+        <v>0.22125200651648699</v>
+      </c>
+      <c r="E77" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>723</v>
+      </c>
+      <c r="B78">
+        <v>30</v>
+      </c>
+      <c r="C78">
+        <v>15</v>
+      </c>
+      <c r="D78">
+        <v>0.221253796904716</v>
+      </c>
+      <c r="E78" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>693</v>
+      </c>
+      <c r="B79">
+        <v>30</v>
+      </c>
+      <c r="C79">
+        <v>20</v>
+      </c>
+      <c r="D79">
+        <v>0.22127170567031901</v>
+      </c>
+      <c r="E79" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>671</v>
+      </c>
+      <c r="B80">
+        <v>30</v>
+      </c>
+      <c r="C80">
+        <v>25</v>
+      </c>
+      <c r="D80">
+        <v>0.22124392541851601</v>
+      </c>
+      <c r="E80" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>663</v>
+      </c>
+      <c r="B81">
+        <v>30</v>
+      </c>
+      <c r="C81">
+        <v>30</v>
+      </c>
+      <c r="D81">
+        <v>0.22124052248620599</v>
+      </c>
+      <c r="E81" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>593</v>
+      </c>
+      <c r="B82">
+        <v>40</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82">
+        <v>0.22236450170070701</v>
+      </c>
+      <c r="E82" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>731</v>
+      </c>
+      <c r="B83">
+        <v>40</v>
+      </c>
+      <c r="C83">
+        <v>6</v>
+      </c>
+      <c r="D83">
+        <v>0.22146229860554401</v>
+      </c>
+      <c r="E83" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>711</v>
+      </c>
+      <c r="B84">
+        <v>40</v>
+      </c>
+      <c r="C84">
+        <v>7</v>
+      </c>
+      <c r="D84">
+        <v>0.221372305522444</v>
+      </c>
+      <c r="E84" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>697</v>
+      </c>
+      <c r="B85">
+        <v>40</v>
+      </c>
+      <c r="C85">
+        <v>8</v>
+      </c>
+      <c r="D85">
+        <v>0.22129291386108299</v>
+      </c>
+      <c r="E85" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>761</v>
+      </c>
+      <c r="B86">
+        <v>40</v>
+      </c>
+      <c r="C86">
+        <v>9</v>
+      </c>
+      <c r="D86">
+        <v>0.22123502226831601</v>
+      </c>
+      <c r="E86" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>667</v>
+      </c>
+      <c r="B87">
+        <v>40</v>
+      </c>
+      <c r="C87">
+        <v>12</v>
+      </c>
+      <c r="D87">
+        <v>0.22122485215552101</v>
+      </c>
+      <c r="E87" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>770</v>
+      </c>
+      <c r="B88">
+        <v>40</v>
+      </c>
+      <c r="C88">
+        <v>15</v>
+      </c>
+      <c r="D88">
+        <v>0.221205172193429</v>
+      </c>
+      <c r="E88" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>768</v>
+      </c>
+      <c r="B89">
+        <v>40</v>
+      </c>
+      <c r="C89">
+        <v>20</v>
+      </c>
+      <c r="D89">
+        <v>0.22126954140021199</v>
+      </c>
+      <c r="E89" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>766</v>
+      </c>
+      <c r="B90">
+        <v>40</v>
+      </c>
+      <c r="C90">
+        <v>25</v>
+      </c>
+      <c r="D90">
+        <v>0.22127405351708199</v>
+      </c>
+      <c r="E90" t="s">
+        <v>767</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:E90">
+    <sortCondition ref="B2:B90"/>
+    <sortCondition ref="C2:C90"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="B4:C11"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20482,13 +24171,13 @@
       </c>
       <c r="C10" s="16">
         <f t="shared" ref="C10:C12" si="1">E10/D10</f>
-        <v>9.8379629629629633E-3</v>
+        <v>9.0663580246913584E-3</v>
       </c>
       <c r="D10">
         <v>5184</v>
       </c>
       <c r="E10">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F10">
         <v>213</v>
@@ -20500,13 +24189,13 @@
       </c>
       <c r="C11" s="16">
         <f t="shared" si="1"/>
-        <v>9.7957828324755098E-3</v>
+        <v>9.6297526149759262E-3</v>
       </c>
       <c r="D11">
         <v>6023</v>
       </c>
       <c r="E11">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -20518,7 +24207,7 @@
       </c>
       <c r="C12" s="16">
         <f t="shared" si="1"/>
-        <v>7.0526215805471124E-3</v>
+        <v>6.9338905775075989E-3</v>
       </c>
       <c r="D12" s="4">
         <f>SUM(D4:D11)</f>
@@ -20526,7 +24215,7 @@
       </c>
       <c r="E12" s="4">
         <f>SUM(E4:E11)</f>
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F12" s="4">
         <f>SUM(F4:F11)</f>
@@ -20554,7 +24243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L209"/>
   <sheetViews>

</xml_diff>